<commit_message>
Sowmya & Kiran | #601 | Modifying training data to accommodate child immunization and vitamin a column changes. Uploading vitamin A dosages
</commit_message>
<xml_diff>
--- a/drishti-tools/upload_forms/examples/10 Training data.xlsx
+++ b/drishti-tools/upload_forms/examples/10 Training data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19400" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="EC register" sheetId="8" r:id="rId1"/>
@@ -1140,7 +1140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="350">
   <si>
     <t>Ashwini</t>
   </si>
@@ -2159,81 +2159,6 @@
     <t>Saanvi</t>
   </si>
   <si>
-    <t>BCG</t>
-  </si>
-  <si>
-    <t>Hep B 0</t>
-  </si>
-  <si>
-    <t>OPV 0</t>
-  </si>
-  <si>
-    <t>OPV 1</t>
-  </si>
-  <si>
-    <t>OPV 2</t>
-  </si>
-  <si>
-    <t>OPV 3</t>
-  </si>
-  <si>
-    <t>Pentavalent 1</t>
-  </si>
-  <si>
-    <t>Pentavalent 2</t>
-  </si>
-  <si>
-    <t>Pentavalent 3</t>
-  </si>
-  <si>
-    <t>Measles</t>
-  </si>
-  <si>
-    <t>DPT Booster 1</t>
-  </si>
-  <si>
-    <t>DPT Booster 2</t>
-  </si>
-  <si>
-    <t>Vit A 1</t>
-  </si>
-  <si>
-    <t>Vit A 2</t>
-  </si>
-  <si>
-    <t>Vit A 3</t>
-  </si>
-  <si>
-    <t>Vit A 4</t>
-  </si>
-  <si>
-    <t>Vit A 5</t>
-  </si>
-  <si>
-    <t>Vit A 6</t>
-  </si>
-  <si>
-    <t>Vit A 7</t>
-  </si>
-  <si>
-    <t>Vit A 8</t>
-  </si>
-  <si>
-    <t>Vit A 9</t>
-  </si>
-  <si>
-    <t>OPV Booster</t>
-  </si>
-  <si>
-    <t>17/02/2013</t>
-  </si>
-  <si>
-    <t>17/03/2013</t>
-  </si>
-  <si>
-    <t>14/04/013</t>
-  </si>
-  <si>
     <t>TT Injection place</t>
   </si>
   <si>
@@ -2247,6 +2172,24 @@
   </si>
   <si>
     <t>Woman survived child birth</t>
+  </si>
+  <si>
+    <t>Immunization</t>
+  </si>
+  <si>
+    <t>Immunization date</t>
+  </si>
+  <si>
+    <t>opv_0</t>
+  </si>
+  <si>
+    <t>opv_1</t>
+  </si>
+  <si>
+    <t>Vitamin A dose</t>
+  </si>
+  <si>
+    <t>Vitamin A date</t>
   </si>
 </sst>
 </file>
@@ -2495,11 +2438,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="228">
+  <cellStyleXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2852,7 +2805,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="228">
+  <cellStyles count="238">
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
@@ -2965,6 +2918,11 @@
     <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -3077,6 +3035,11 @@
     <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet2" xfId="2"/>
     <cellStyle name="Normal_Sheet3" xfId="1"/>
@@ -10167,10 +10130,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10178,12 +10141,11 @@
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="10" customFormat="1">
+    <row r="1" spans="1:9" s="10" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -10194,46 +10156,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>343</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="J1" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="17" t="s">
         <v>141</v>
       </c>
@@ -10243,21 +10172,18 @@
       <c r="C2" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="D2" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>316</v>
+      </c>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-    </row>
-    <row r="3" spans="1:16">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="17" t="s">
         <v>119</v>
       </c>
@@ -10268,26 +10194,17 @@
         <v>29230030071</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>271</v>
+        <v>347</v>
       </c>
       <c r="E3" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="F3" s="34" t="s">
-        <v>271</v>
-      </c>
+      <c r="F3" s="34"/>
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
       <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-    </row>
-    <row r="4" spans="1:16">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -10298,26 +10215,17 @@
         <v>29230030071</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>269</v>
+        <v>346</v>
       </c>
       <c r="E4" s="34" t="s">
         <v>269</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>269</v>
-      </c>
+      <c r="F4" s="34"/>
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
       <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-    </row>
-    <row r="5" spans="1:16">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>280</v>
       </c>
@@ -10328,26 +10236,17 @@
         <v>29230030068</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>284</v>
+        <v>347</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="F5" s="34" t="s">
-        <v>284</v>
-      </c>
+      <c r="F5" s="34"/>
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
       <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-    </row>
-    <row r="6" spans="1:16">
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -10358,26 +10257,17 @@
         <v>59</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>285</v>
+        <v>346</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>285</v>
       </c>
-      <c r="F6" s="34" t="s">
-        <v>285</v>
-      </c>
+      <c r="F6" s="34"/>
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-    </row>
-    <row r="7" spans="1:16">
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>281</v>
       </c>
@@ -10388,26 +10278,17 @@
         <v>59</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>267</v>
+        <v>347</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="F7" s="34" t="s">
-        <v>267</v>
-      </c>
+      <c r="F7" s="34"/>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-    </row>
-    <row r="8" spans="1:16">
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="17" t="s">
         <v>61</v>
       </c>
@@ -10418,38 +10299,17 @@
         <v>59</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>316</v>
+        <v>346</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>316</v>
       </c>
-      <c r="F8" s="34" t="s">
-        <v>316</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>361</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>362</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="J8" s="34" t="s">
-        <v>361</v>
-      </c>
-      <c r="K8" s="34" t="s">
-        <v>362</v>
-      </c>
-      <c r="L8" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="17" t="s">
         <v>77</v>
       </c>
@@ -10459,21 +10319,18 @@
       <c r="C9" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="D9" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>271</v>
+      </c>
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-    </row>
-    <row r="10" spans="1:16">
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="17" t="s">
         <v>121</v>
       </c>
@@ -10483,21 +10340,18 @@
       <c r="C10" s="35">
         <v>29230030071</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
+      <c r="D10" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>269</v>
+      </c>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
       <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-    </row>
-    <row r="11" spans="1:16">
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="17" t="s">
         <v>133</v>
       </c>
@@ -10507,21 +10361,18 @@
       <c r="C11" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
+      <c r="D11" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>284</v>
+      </c>
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
       <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-    </row>
-    <row r="12" spans="1:16">
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="17" t="s">
         <v>173</v>
       </c>
@@ -10531,21 +10382,18 @@
       <c r="C12" s="35">
         <v>29230030070</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
+      <c r="D12" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>285</v>
+      </c>
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-    </row>
-    <row r="13" spans="1:16">
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="27" t="s">
         <v>180</v>
       </c>
@@ -10555,21 +10403,18 @@
       <c r="C13" s="35">
         <v>29230030070</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
+      <c r="D13" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>267</v>
+      </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-    </row>
-    <row r="14" spans="1:16">
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="27" t="s">
         <v>216</v>
       </c>
@@ -10579,21 +10424,18 @@
       <c r="C14" s="35">
         <v>29230030070</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
+      <c r="D14" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>316</v>
+      </c>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
-    </row>
-    <row r="15" spans="1:16">
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="27" t="s">
         <v>99</v>
       </c>
@@ -10603,21 +10445,18 @@
       <c r="C15" s="35">
         <v>29230030068</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
+      <c r="D15" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>271</v>
+      </c>
       <c r="F15" s="34"/>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-    </row>
-    <row r="16" spans="1:16">
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="17" t="s">
         <v>200</v>
       </c>
@@ -10627,21 +10466,18 @@
       <c r="C16" s="35">
         <v>29230030070</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
+      <c r="D16" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>269</v>
+      </c>
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-    </row>
-    <row r="17" spans="1:16">
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="17" t="s">
         <v>203</v>
       </c>
@@ -10651,21 +10487,18 @@
       <c r="C17" s="35">
         <v>29230030070</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
+      <c r="D17" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>284</v>
+      </c>
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
-    </row>
-    <row r="18" spans="1:16">
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="17" t="s">
         <v>234</v>
       </c>
@@ -10675,21 +10508,18 @@
       <c r="C18" s="35">
         <v>29230030070</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
+      <c r="D18" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>285</v>
+      </c>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-    </row>
-    <row r="19" spans="1:16">
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="17" t="s">
         <v>185</v>
       </c>
@@ -10699,21 +10529,18 @@
       <c r="C19" s="35">
         <v>29230030070</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
+      <c r="D19" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>267</v>
+      </c>
       <c r="F19" s="34"/>
       <c r="G19" s="34"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-    </row>
-    <row r="20" spans="1:16">
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="27" t="s">
         <v>237</v>
       </c>
@@ -10723,21 +10550,18 @@
       <c r="C20" s="35">
         <v>29230030070</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
+      <c r="D20" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>316</v>
+      </c>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
       <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-    </row>
-    <row r="21" spans="1:16">
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="17" t="s">
         <v>145</v>
       </c>
@@ -10747,22 +10571,16 @@
       <c r="C21" s="35">
         <v>29230030070</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
+      <c r="D21" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>316</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -10773,10 +10591,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10785,7 +10603,7 @@
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1">
+    <row r="1" spans="1:5" s="14" customFormat="1" ht="28">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -10796,34 +10614,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="17" t="s">
         <v>141</v>
       </c>
@@ -10833,8 +10630,14 @@
       <c r="C2" s="42" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="17" t="s">
         <v>119</v>
       </c>
@@ -10844,8 +10647,14 @@
       <c r="C3" s="35">
         <v>29230030071</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -10855,8 +10664,14 @@
       <c r="C4" s="35">
         <v>29230030071</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>280</v>
       </c>
@@ -10866,8 +10681,14 @@
       <c r="C5" s="35">
         <v>29230030068</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -10877,8 +10698,14 @@
       <c r="C6" s="18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>281</v>
       </c>
@@ -10888,8 +10715,14 @@
       <c r="C7" s="18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="17" t="s">
         <v>61</v>
       </c>
@@ -10899,8 +10732,14 @@
       <c r="C8" s="18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="17" t="s">
         <v>77</v>
       </c>
@@ -10910,8 +10749,14 @@
       <c r="C9" s="18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="17" t="s">
         <v>121</v>
       </c>
@@ -10921,8 +10766,14 @@
       <c r="C10" s="35">
         <v>29230030071</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="17" t="s">
         <v>133</v>
       </c>
@@ -10932,8 +10783,14 @@
       <c r="C11" s="20" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="17" t="s">
         <v>173</v>
       </c>
@@ -10943,8 +10800,14 @@
       <c r="C12" s="35">
         <v>29230030070</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="27" t="s">
         <v>180</v>
       </c>
@@ -10954,8 +10817,14 @@
       <c r="C13" s="35">
         <v>29230030070</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="27" t="s">
         <v>216</v>
       </c>
@@ -10965,8 +10834,14 @@
       <c r="C14" s="35">
         <v>29230030070</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="27" t="s">
         <v>99</v>
       </c>
@@ -10976,8 +10851,14 @@
       <c r="C15" s="35">
         <v>29230030068</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="17" t="s">
         <v>200</v>
       </c>
@@ -10987,8 +10868,14 @@
       <c r="C16" s="35">
         <v>29230030070</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="17" t="s">
         <v>203</v>
       </c>
@@ -10998,8 +10885,14 @@
       <c r="C17" s="35">
         <v>29230030070</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="17" t="s">
         <v>234</v>
       </c>
@@ -11009,8 +10902,14 @@
       <c r="C18" s="35">
         <v>29230030070</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="17" t="s">
         <v>185</v>
       </c>
@@ -11020,8 +10919,14 @@
       <c r="C19" s="35">
         <v>29230030070</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="27" t="s">
         <v>237</v>
       </c>
@@ -11031,8 +10936,14 @@
       <c r="C20" s="35">
         <v>29230030070</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="17" t="s">
         <v>145</v>
       </c>
@@ -11042,9 +10953,16 @@
       <c r="C21" s="35">
         <v>29230030070</v>
       </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>316</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -11058,7 +10976,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -11564,7 +11482,7 @@
         <v>52</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>364</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -11578,7 +11496,7 @@
         <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
       <c r="E2" s="43">
         <v>41445</v>
@@ -11598,7 +11516,7 @@
         <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>366</v>
+        <v>341</v>
       </c>
       <c r="E3" s="43">
         <v>41446</v>
@@ -11618,7 +11536,7 @@
         <v>159</v>
       </c>
       <c r="D4" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
       <c r="E4" s="43">
         <v>41447</v>
@@ -11638,7 +11556,7 @@
         <v>159</v>
       </c>
       <c r="D5" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
       <c r="E5" s="43">
         <v>41448</v>
@@ -11658,7 +11576,7 @@
         <v>159</v>
       </c>
       <c r="D6" t="s">
-        <v>366</v>
+        <v>341</v>
       </c>
       <c r="E6" s="43">
         <v>41449</v>
@@ -11678,7 +11596,7 @@
         <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
       <c r="E7" s="43">
         <v>41450</v>
@@ -11698,7 +11616,7 @@
         <v>159</v>
       </c>
       <c r="D8" t="s">
-        <v>367</v>
+        <v>342</v>
       </c>
       <c r="E8" s="43">
         <v>41451</v>
@@ -11718,7 +11636,7 @@
         <v>159</v>
       </c>
       <c r="D9" t="s">
-        <v>367</v>
+        <v>342</v>
       </c>
       <c r="E9" s="43">
         <v>41452</v>
@@ -11735,7 +11653,7 @@
         <v>159</v>
       </c>
       <c r="D10" t="s">
-        <v>367</v>
+        <v>342</v>
       </c>
       <c r="E10" s="43">
         <v>41453</v>
@@ -11755,7 +11673,7 @@
         <v>238</v>
       </c>
       <c r="D11" t="s">
-        <v>366</v>
+        <v>341</v>
       </c>
       <c r="E11" s="43">
         <v>41454</v>
@@ -12256,8 +12174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -12311,7 +12229,7 @@
         <v>249</v>
       </c>
       <c r="N1" s="30" t="s">
-        <v>368</v>
+        <v>343</v>
       </c>
       <c r="O1" s="30" t="s">
         <v>248</v>
@@ -12724,7 +12642,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>